<commit_message>
Modified the countries list for EU RED
</commit_message>
<xml_diff>
--- a/dcs/rfid/android/EU-RED-Countries.xlsx
+++ b/dcs/rfid/android/EU-RED-Countries.xlsx
@@ -2,16 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ng1388\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ng1388\techdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D66F39A3-AF5C-4064-A6BE-39358D59722B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDC88BAA-902E-4143-AB09-ABB33918758D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{55205051-B463-41AE-A48E-ADE784D169E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55205051-B463-41AE-A48E-ADE784D169E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,9 +71,6 @@
     <t>Cyprus</t>
   </si>
   <si>
-    <t>Czechia</t>
-  </si>
-  <si>
     <t>Denmark</t>
   </si>
   <si>
@@ -150,9 +146,6 @@
     <t>Sweden.</t>
   </si>
   <si>
-    <t>Swizerland</t>
-  </si>
-  <si>
     <t>Turkey</t>
   </si>
   <si>
@@ -199,6 +192,12 @@
   </si>
   <si>
     <t>Vatican City</t>
+  </si>
+  <si>
+    <t>Czechia(Czech Republic)</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
   </si>
 </sst>
 </file>
@@ -633,19 +632,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2837365-49C2-4A4F-97A8-2A57BE97AF41}">
   <dimension ref="B2:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -679,7 +678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -696,7 +695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -713,7 +712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -730,7 +729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>5</v>
       </c>
@@ -747,12 +746,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
@@ -764,12 +763,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
@@ -781,12 +780,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>6</v>
@@ -798,12 +797,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>6</v>
@@ -815,12 +814,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>6</v>
@@ -832,46 +831,46 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>13</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>6</v>
@@ -883,12 +882,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>6</v>
@@ -900,46 +899,46 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="4">
-        <v>16</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="D18" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>6</v>
@@ -951,12 +950,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>6</v>
@@ -968,12 +967,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>19</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>6</v>
@@ -985,63 +984,63 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>20</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>21</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>22</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>23</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>6</v>
@@ -1053,29 +1052,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>24</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>25</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>6</v>
@@ -1087,12 +1086,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>26</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>6</v>
@@ -1104,12 +1103,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>27</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>6</v>
@@ -1121,12 +1120,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>28</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>6</v>
@@ -1138,12 +1137,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>29</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>6</v>
@@ -1155,12 +1154,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>30</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>6</v>
@@ -1172,12 +1171,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>31</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>6</v>
@@ -1189,276 +1188,276 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
         <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>33</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>34</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <v>35</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>36</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>37</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="4">
         <v>38</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="4">
         <v>39</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="4">
         <v>40</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>41</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="4">
         <v>42</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>43</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="4">
         <v>44</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
         <v>45</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="4">
         <v>46</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="4">
         <v>47</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>